<commit_message>
new structure for data files
</commit_message>
<xml_diff>
--- a/storage/data/Users.xlsx
+++ b/storage/data/Users.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikola\Desktop\Foodvine\testing\Auto_tests\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nikola\Desktop\Foodvine\testing\Auto_tests\foodvine-ga\storage\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE67412B-72FA-4BF8-AD82-F25B247146AE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92D58068-1E4F-4364-9325-5BFDB6D2BAE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,13 +31,13 @@
     <t>password</t>
   </si>
   <si>
-    <t>1234Test</t>
-  </si>
-  <si>
     <t>testnikola1</t>
   </si>
   <si>
     <t>testnikola1@gmail.com</t>
+  </si>
+  <si>
+    <t>1234Tests</t>
   </si>
 </sst>
 </file>
@@ -369,7 +369,7 @@
   <dimension ref="A1:C2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,13 +392,13 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>3</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" t="s">
         <v>5</v>
-      </c>
-      <c r="C2" t="s">
-        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>